<commit_message>
Fix json file parse
</commit_message>
<xml_diff>
--- a/Data/节奏与升级系统表格_加入敌人权重.xlsx
+++ b/Data/节奏与升级系统表格_加入敌人权重.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Godot\fox\Data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0CF0A5A-DBEE-4919-9B56-92812D00005C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -85,12 +79,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -98,15 +92,8 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -156,21 +143,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -208,7 +187,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -242,7 +221,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -277,10 +255,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -453,27 +430,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="1" width="18.125" customWidth="1"/>
-    <col min="2" max="2" width="20.375" customWidth="1"/>
-    <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="4" max="4" width="12.75" customWidth="1"/>
-    <col min="5" max="5" width="17" customWidth="1"/>
-    <col min="6" max="6" width="16.375" customWidth="1"/>
-    <col min="7" max="7" width="13.125" customWidth="1"/>
-    <col min="8" max="8" width="18.5" customWidth="1"/>
-    <col min="15" max="15" width="61.125" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -520,7 +484,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:15">
       <c r="A2">
         <v>0</v>
       </c>
@@ -546,7 +510,7 @@
         <v>2</v>
       </c>
       <c r="I2">
-        <v>0.33500000000000002</v>
+        <v>0.335</v>
       </c>
       <c r="J2">
         <v>10</v>
@@ -567,7 +531,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:15">
       <c r="A3">
         <v>10</v>
       </c>
@@ -587,16 +551,16 @@
         <v>0.48</v>
       </c>
       <c r="G3">
-        <v>0.69</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="H3">
         <v>2.08</v>
       </c>
       <c r="I3">
-        <v>0.33200000000000002</v>
+        <v>0.332</v>
       </c>
       <c r="J3">
-        <v>9.6999999999999993</v>
+        <v>9.699999999999999</v>
       </c>
       <c r="K3">
         <v>1</v>
@@ -614,7 +578,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:15">
       <c r="A4">
         <v>20</v>
       </c>
@@ -640,7 +604,7 @@
         <v>2.13</v>
       </c>
       <c r="I4">
-        <v>0.33300000000000002</v>
+        <v>0.333</v>
       </c>
       <c r="J4">
         <v>9.4</v>
@@ -661,7 +625,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:15">
       <c r="A5">
         <v>30</v>
       </c>
@@ -681,13 +645,13 @@
         <v>0.46</v>
       </c>
       <c r="G5">
-        <v>1.1100000000000001</v>
+        <v>1.11</v>
       </c>
       <c r="H5">
         <v>2.17</v>
       </c>
       <c r="I5">
-        <v>0.51200000000000001</v>
+        <v>0.512</v>
       </c>
       <c r="J5">
         <v>9.1</v>
@@ -708,7 +672,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:15">
       <c r="A6">
         <v>40</v>
       </c>
@@ -755,7 +719,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:15">
       <c r="A7">
         <v>50</v>
       </c>
@@ -784,7 +748,7 @@
         <v>1.008</v>
       </c>
       <c r="J7">
-        <v>8.1999999999999993</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="K7">
         <v>2</v>
@@ -802,7 +766,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:15">
       <c r="A8">
         <v>60</v>
       </c>
@@ -828,7 +792,7 @@
         <v>4.88</v>
       </c>
       <c r="I8">
-        <v>0.68200000000000005</v>
+        <v>0.6820000000000001</v>
       </c>
       <c r="J8">
         <v>7.9</v>
@@ -849,12 +813,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:15">
       <c r="A9">
         <v>70</v>
       </c>
       <c r="B9">
-        <v>2.2999999999999998</v>
+        <v>2.3</v>
       </c>
       <c r="C9">
         <v>4</v>
@@ -875,7 +839,7 @@
         <v>5</v>
       </c>
       <c r="I9">
-        <v>0.69599999999999995</v>
+        <v>0.696</v>
       </c>
       <c r="J9">
         <v>7.6</v>
@@ -896,12 +860,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:15">
       <c r="A10">
         <v>80</v>
       </c>
       <c r="B10">
-        <v>2.2000000000000002</v>
+        <v>2.2</v>
       </c>
       <c r="C10">
         <v>4</v>
@@ -943,7 +907,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:15">
       <c r="A11">
         <v>90</v>
       </c>
@@ -990,7 +954,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:15">
       <c r="A12">
         <v>100</v>
       </c>
@@ -1037,7 +1001,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:15">
       <c r="A13">
         <v>110</v>
       </c>
@@ -1084,7 +1048,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:15">
       <c r="A14">
         <v>120</v>
       </c>
@@ -1107,10 +1071,10 @@
         <v>10</v>
       </c>
       <c r="H14">
-        <v>9.3800000000000008</v>
+        <v>9.380000000000001</v>
       </c>
       <c r="I14">
-        <v>1.0660000000000001</v>
+        <v>1.066</v>
       </c>
       <c r="J14">
         <v>6.1</v>
@@ -1131,7 +1095,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:15">
       <c r="A15">
         <v>130</v>
       </c>
@@ -1157,7 +1121,7 @@
         <v>10</v>
       </c>
       <c r="I15">
-        <v>1.0589999999999999</v>
+        <v>1.059</v>
       </c>
       <c r="J15">
         <v>5.8</v>
@@ -1178,7 +1142,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:15">
       <c r="A16">
         <v>140</v>
       </c>
@@ -1195,7 +1159,7 @@
         <v>3</v>
       </c>
       <c r="F16">
-        <v>0.28999999999999998</v>
+        <v>0.29</v>
       </c>
       <c r="G16">
         <v>15</v>
@@ -1204,7 +1168,7 @@
         <v>10.34</v>
       </c>
       <c r="I16">
-        <v>1.4510000000000001</v>
+        <v>1.451</v>
       </c>
       <c r="J16">
         <v>5.5</v>
@@ -1225,7 +1189,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:15">
       <c r="A17">
         <v>150</v>
       </c>
@@ -1242,16 +1206,16 @@
         <v>3</v>
       </c>
       <c r="F17">
-        <v>0.28000000000000003</v>
+        <v>0.28</v>
       </c>
       <c r="G17">
-        <v>18.670000000000002</v>
+        <v>18.67</v>
       </c>
       <c r="H17">
         <v>10.71</v>
       </c>
       <c r="I17">
-        <v>1.7430000000000001</v>
+        <v>1.743</v>
       </c>
       <c r="J17">
         <v>5.5</v>
@@ -1273,7 +1237,6 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>